<commit_message>
//정협 2017-11-16 1.EnemyChracter DropItem 2.Prefab ITem 추가
</commit_message>
<xml_diff>
--- a/Assets/Resources/Table/DataTable.xlsx
+++ b/Assets/Resources/Table/DataTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14190" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14190" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -199,10 +199,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>armor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>weapon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -420,6 +416,10 @@
   </si>
   <si>
     <t>HandAxe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accessori</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -838,10 +838,10 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
@@ -859,7 +859,7 @@
         <v>20</v>
       </c>
       <c r="K1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -975,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5">
         <v>-1</v>
@@ -1010,7 +1010,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1045,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -1080,7 +1080,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1115,7 +1115,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9">
         <v>-1</v>
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10">
         <v>-1</v>
@@ -1185,7 +1185,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1220,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13">
         <v>-1</v>
@@ -1290,7 +1290,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1325,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15">
         <v>-1</v>
@@ -1360,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16">
         <v>-1</v>
@@ -1395,7 +1395,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -1465,7 +1465,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1500,7 +1500,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20">
         <v>-1</v>
@@ -1535,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21">
         <v>-1</v>
@@ -1570,7 +1570,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22">
         <v>10</v>
@@ -1605,7 +1605,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23">
         <v>-1</v>
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24">
         <v>-1</v>
@@ -1675,7 +1675,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1710,7 +1710,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D26">
         <v>-1</v>
@@ -1745,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27">
         <v>-1</v>
@@ -1780,7 +1780,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -2022,8 +2022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2045,10 +2045,10 @@
         <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
         <v>38</v>
@@ -2066,34 +2066,34 @@
         <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
         <v>43</v>
       </c>
       <c r="K1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
-        <v>48</v>
-      </c>
       <c r="P1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
-        <v>54</v>
-      </c>
       <c r="R1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -2104,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <v>8000</v>
@@ -2125,13 +2125,13 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>-1</v>
+        <v>14</v>
       </c>
       <c r="K2">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="L2">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -2160,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3">
         <v>4000</v>
@@ -2181,13 +2181,13 @@
         <v>12</v>
       </c>
       <c r="J3">
-        <v>-1</v>
+        <v>25</v>
       </c>
       <c r="K3">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="L3">
-        <v>-1</v>
+        <v>26</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -2216,7 +2216,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4">
         <v>9000</v>
@@ -2237,13 +2237,13 @@
         <v>8</v>
       </c>
       <c r="J4">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="K4">
-        <v>-1</v>
+        <v>18</v>
       </c>
       <c r="L4">
-        <v>-1</v>
+        <v>20</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -2272,7 +2272,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5">
         <v>4000</v>
@@ -2293,13 +2293,13 @@
         <v>12</v>
       </c>
       <c r="J5">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>-1</v>
+        <v>21</v>
       </c>
       <c r="L5">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -2328,7 +2328,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6">
         <v>20000</v>
@@ -2349,13 +2349,13 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="K6">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="L6">
-        <v>-1</v>
+        <v>12</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -2384,7 +2384,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7">
         <v>2000</v>
@@ -2405,13 +2405,13 @@
         <v>13</v>
       </c>
       <c r="J7">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="K7">
         <v>-1</v>
       </c>
       <c r="L7">
-        <v>-1</v>
+        <v>17</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -2440,7 +2440,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8">
         <v>4000</v>
@@ -2461,13 +2461,13 @@
         <v>10</v>
       </c>
       <c r="J8">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="K8">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="L8">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -2496,7 +2496,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>2500</v>
@@ -2517,13 +2517,13 @@
         <v>9</v>
       </c>
       <c r="J9">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="K9">
         <v>-1</v>
       </c>
       <c r="L9">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -2552,7 +2552,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>3000</v>
@@ -2573,13 +2573,13 @@
         <v>9</v>
       </c>
       <c r="J10">
-        <v>-1</v>
+        <v>22</v>
       </c>
       <c r="K10">
-        <v>-1</v>
+        <v>21</v>
       </c>
       <c r="L10">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -2608,7 +2608,7 @@
         <v>999</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2650,7 +2650,7 @@
         <v>3000</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -2686,28 +2686,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
       <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>63</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>